<commit_message>
Final update of the Actual Timeline
Comments on what has been done in the synoptic time period in respective weeks. General Comments at the bottom
</commit_message>
<xml_diff>
--- a/Doc/Actual Timeline.xlsx
+++ b/Doc/Actual Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\OneDrive\Desktop\Assignment Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C667D41-1723-43B2-89D5-2AC00BFFA461}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A184DAF4-14A3-4B0C-A6B1-AEFCDA8C55C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BC6927A6-B481-4204-96EC-378E96DEA29F}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,8 +34,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E30FEF6A-71F6-44BE-9BDD-F528367F3658}</author>
+    <author>tc={AC5B5D3A-EA28-4056-979E-C84A8E96C9C5}</author>
+    <author>tc={D44CC025-7AD6-41CE-AD80-931AA4B1BD95}</author>
+  </authors>
+  <commentList>
+    <comment ref="R18" authorId="0" shapeId="0" xr:uid="{E30FEF6A-71F6-44BE-9BDD-F528367F3658}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tried adding log files. Location in paper: Limitation</t>
+      </text>
+    </comment>
+    <comment ref="R21" authorId="1" shapeId="0" xr:uid="{AC5B5D3A-EA28-4056-979E-C84A8E96C9C5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed Intro questions, planning hypothesis, added limitations and improvements.</t>
+      </text>
+    </comment>
+    <comment ref="S21" authorId="2" shapeId="0" xr:uid="{D44CC025-7AD6-41CE-AD80-931AA4B1BD95}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mild rewording of conclusion, added extenstions, more text in findings</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>WP</t>
   </si>
@@ -142,6 +179,54 @@
   </si>
   <si>
     <t>IEEE Paper</t>
+  </si>
+  <si>
+    <t>Synoptic Wk1</t>
+  </si>
+  <si>
+    <t>Synoptic Wk2</t>
+  </si>
+  <si>
+    <t>Editing of Intro &amp; Concl</t>
+  </si>
+  <si>
+    <t>Tweaking of sections</t>
+  </si>
+  <si>
+    <t>Log File Addition</t>
+  </si>
+  <si>
+    <t>Extra Comments</t>
+  </si>
+  <si>
+    <t>Log Files (XML/CSV)</t>
+  </si>
+  <si>
+    <t>Could not be implemented due to outdated codes found</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Changed questions, added hypothesis.</t>
+  </si>
+  <si>
+    <t>Added extention, limitation, improvement. Reworded slightly.</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
+    <t>Added intext citations instead of leaving only numbers.</t>
+  </si>
+  <si>
+    <t>Findings</t>
+  </si>
+  <si>
+    <t>Added few more information that was collected.</t>
   </si>
 </sst>
 </file>
@@ -230,6 +315,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Nicolai Caruana" id="{12581D0C-695B-4641-9A86-DB6525D2D9CA}" userId="aa26a6eefa8db701" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,21 +618,37 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="R18" dT="2021-06-25T13:45:39.18" personId="{12581D0C-695B-4641-9A86-DB6525D2D9CA}" id="{E30FEF6A-71F6-44BE-9BDD-F528367F3658}">
+    <text>Tried adding log files. Location in paper: Limitation</text>
+  </threadedComment>
+  <threadedComment ref="R21" dT="2021-06-24T11:21:07.02" personId="{12581D0C-695B-4641-9A86-DB6525D2D9CA}" id="{AC5B5D3A-EA28-4056-979E-C84A8E96C9C5}">
+    <text>Changed Intro questions, planning hypothesis, added limitations and improvements.</text>
+  </threadedComment>
+  <threadedComment ref="S21" dT="2021-06-25T13:57:55.87" personId="{12581D0C-695B-4641-9A86-DB6525D2D9CA}" id="{D44CC025-7AD6-41CE-AD80-931AA4B1BD95}">
+    <text>Mild rewording of conclusion, added extenstions, more text in findings</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA4C591-2AC8-453F-BE22-3A94064630EE}">
-  <dimension ref="A1:P21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA4C591-2AC8-453F-BE22-3A94064630EE}">
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,12 +697,18 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -605,19 +718,19 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -627,7 +740,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -635,7 +748,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -643,7 +756,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -652,13 +765,13 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -666,14 +779,14 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -683,28 +796,32 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R18" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -712,8 +829,63 @@
         <v>35</v>
       </c>
       <c r="P21" s="6"/>
+      <c r="R21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>